<commit_message>
Changed structure of FSH files to new proposed structure.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Pedigree.xlsx
+++ b/docs/StructureDefinition-Pedigree.xlsx
@@ -1422,16 +1422,16 @@
 </t>
   </si>
   <si>
-    <t>reasonCollected</t>
-  </si>
-  <si>
-    <t>Reason collected</t>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>Reason</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
     &lt;system value="http://ga4gh-cp.github.io/pedigree-fhir-ig/CodeSystem/SectionType"/&gt;
-    &lt;code value="reasonCollected"/&gt;
+    &lt;code value="reason"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>
@@ -1642,7 +1642,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="37.9609375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="15.30078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.52734375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>

</xml_diff>